<commit_message>
Small update to Framework survey name
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85147AE-13BC-40B5-A8A2-8449F6C396CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92800BF-0075-4FAA-9994-78C35621B918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="206">
   <si>
     <t>clause</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Bandim Test App</t>
+  </si>
+  <si>
+    <t>App de Teste Bandim</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1187,7 @@
         <v>204</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>